<commit_message>
- Implemented basic functionality for single user usage.
</commit_message>
<xml_diff>
--- a/presenze.xlsx
+++ b/presenze.xlsx
@@ -1658,13 +1658,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2357,13 +2357,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3050,13 +3050,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3749,13 +3749,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3913,9 +3913,21 @@
       <c r="B12" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="C12" s="24" t="n"/>
-      <c r="D12" s="24" t="n"/>
-      <c r="E12" s="25" t="n"/>
+      <c r="C12" s="24" t="inlineStr">
+        <is>
+          <t>2,50</t>
+        </is>
+      </c>
+      <c r="D12" s="24" t="inlineStr">
+        <is>
+          <t>5,50</t>
+        </is>
+      </c>
+      <c r="E12" s="25" t="inlineStr">
+        <is>
+          <t>5,75</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="26" t="inlineStr">
@@ -4442,13 +4454,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5145,13 +5157,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5842,13 +5854,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6541,13 +6553,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7234,13 +7246,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7933,13 +7945,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8632,13 +8644,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9325,13 +9337,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>